<commit_message>
Separação Japones e Mandarim
</commit_message>
<xml_diff>
--- a/ExperimentoLinguistica/wwwroot/lista.xlsx
+++ b/ExperimentoLinguistica/wwwroot/lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael.pinheiro\source\repos\ExperimentoLinguistica\ExperimentoLinguistica\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07CC54F1-2A8C-42E4-BDD1-3F1B3E674B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D39A3-5911-4A14-9FC1-F6DAFCBBEB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-84" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9B563BA9-7241-4ADD-900D-019F750A50B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
   <si>
     <t>Alvo</t>
   </si>
@@ -108,14 +108,31 @@
   </si>
   <si>
     <t>打电话</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>Japones</t>
+  </si>
+  <si>
+    <t>Mandarim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -143,8 +160,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,18 +497,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E175FA4E-D289-4A8E-AEAA-346C62735FDD}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,8 +522,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -517,8 +539,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -531,8 +556,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -545,8 +573,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -559,8 +590,11 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -573,8 +607,11 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -587,8 +624,11 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -601,8 +641,11 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -615,8 +658,11 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -629,8 +675,11 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -643,8 +692,183 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Guid no nome do arquivo e lista de resultado de avaliacao
</commit_message>
<xml_diff>
--- a/ExperimentoLinguistica/wwwroot/lista.xlsx
+++ b/ExperimentoLinguistica/wwwroot/lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael.pinheiro\source\repos\ExperimentoLinguistica\ExperimentoLinguistica\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D39A3-5911-4A14-9FC1-F6DAFCBBEB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D46BF-EA33-4C5C-BB98-A28EC43452DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-84" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9B563BA9-7241-4ADD-900D-019F750A50B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="24">
   <si>
     <t>Alvo</t>
   </si>
@@ -59,9 +59,6 @@
     <t>ytf</t>
   </si>
   <si>
-    <t>tkqb</t>
-  </si>
-  <si>
     <t>jaddkks</t>
   </si>
   <si>
@@ -71,15 +68,6 @@
     <t>rancho</t>
   </si>
   <si>
-    <t>rtw</t>
-  </si>
-  <si>
-    <t>dxcf</t>
-  </si>
-  <si>
-    <t>gjfedks</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -95,21 +83,9 @@
     <t>看</t>
   </si>
   <si>
-    <t>睡觉</t>
-  </si>
-  <si>
     <t>没关系</t>
   </si>
   <si>
-    <t>做</t>
-  </si>
-  <si>
-    <t>下雨</t>
-  </si>
-  <si>
-    <t>打电话</t>
-  </si>
-  <si>
     <t>Idioma</t>
   </si>
   <si>
@@ -117,6 +93,21 @@
   </si>
   <si>
     <t>Mandarim</t>
+  </si>
+  <si>
+    <t>Lista</t>
+  </si>
+  <si>
+    <t>Aquela Parada 2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>&amp;&amp;&amp;&amp;</t>
   </si>
 </sst>
 </file>
@@ -497,19 +488,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E175FA4E-D289-4A8E-AEAA-346C62735FDD}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A19" sqref="A19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,351 +511,431 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
         <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Alterar mascara para 6 caracteres - Revisao do SOAs - ID com 8 caracteres -Teste de similaridade para 7 pontos - Aumento de fonte
</commit_message>
<xml_diff>
--- a/ExperimentoLinguistica/wwwroot/lista.xlsx
+++ b/ExperimentoLinguistica/wwwroot/lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael.pinheiro\source\repos\ExperimentoLinguistica\ExperimentoLinguistica\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D46BF-EA33-4C5C-BB98-A28EC43452DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074D1898-F8A3-4243-82CB-B2A7EB96E18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-84" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9B563BA9-7241-4ADD-900D-019F750A50B7}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>#######</t>
-  </si>
-  <si>
     <t>苹果</t>
   </si>
   <si>
@@ -107,7 +104,10 @@
     <t>B</t>
   </si>
   <si>
-    <t>&amp;&amp;&amp;&amp;</t>
+    <t>######</t>
+  </si>
+  <si>
+    <t>&amp;&amp;&amp;&amp;&amp;&amp;</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:G19"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,27 +511,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -540,21 +540,21 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -563,21 +563,21 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -586,21 +586,21 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -609,21 +609,21 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -632,21 +632,21 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -655,21 +655,21 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -678,21 +678,21 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -701,22 +701,22 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -725,21 +725,21 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -748,21 +748,21 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -771,21 +771,21 @@
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -794,21 +794,21 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -817,21 +817,21 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
@@ -840,21 +840,21 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -863,21 +863,21 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -886,21 +886,21 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
@@ -909,21 +909,21 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
@@ -932,10 +932,10 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>